<commit_message>
Added the readme.md file
</commit_message>
<xml_diff>
--- a/lazyGenius.xlsx
+++ b/lazyGenius.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
   <si>
     <t>Team Name</t>
   </si>
@@ -234,21 +234,6 @@
   </si>
   <si>
     <t>43.0</t>
-  </si>
-  <si>
-    <t>UpcomingXI</t>
-  </si>
-  <si>
-    <t>3,395.5</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>134</t>
-  </si>
-  <si>
-    <t>16.0</t>
   </si>
   <si>
     <t>Vammy XI</t>
@@ -661,88 +646,78 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="B17" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="C17" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="D17" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E17" t="s" s="2">
-        <v>78</v>
-      </c>
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s" s="2">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E19" t="s" s="2">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E20" t="s" s="2">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D21" t="s" s="2">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s" s="2">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>